<commit_message>
fingers crossed, ABUS template adjustments
</commit_message>
<xml_diff>
--- a/Mamm_Template_ABUS.xlsx
+++ b/Mamm_Template_ABUS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usradiology-my.sharepoint.com/personal/joshua_mcdonald_usradiology_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A549B7B-4848-4AAA-9644-DE22D79D29E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{3A549B7B-4848-4AAA-9644-DE22D79D29E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDC46753-5E0B-4381-B9E6-CD466FBD2315}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="777" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -872,7 +872,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C7">
         <f>Ballantyne!C7+Blakeney!C7+Huntersville!C7+Matthews!C7+McDowell!C7+MCP!C7+MMP!C7+Mobile!C7+Monroe!C7+Mooresville!C7+Pineville!C7+Prosperity!C7+'Rock Hill'!C7+Rosedale!C7+Southpark!C7+'Steele Creek'!C7+'Union West'!C7+University!C7</f>
@@ -928,7 +928,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <f>Ballantyne!C8+Blakeney!C8+Huntersville!C8+Matthews!C8+McDowell!C8+MCP!C8+MMP!C8+Mobile!C8+Monroe!C8+Mooresville!C8+Pineville!C8+Prosperity!C8+'Rock Hill'!C8+Rosedale!C8+Southpark!C8+'Steele Creek'!C8+'Union West'!C8+University!C8</f>
@@ -1714,2022 +1714,6 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:N21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="14" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:N21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="14" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:N21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="14" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:N21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="14" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:N21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="14" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:N21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="14" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:N21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="14" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:N21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="14" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:N21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="14" width="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3830,7 +1814,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -3838,7 +1822,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -3950,12 +1934,1788 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="14" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="14" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="14" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="14" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="14" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="14" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="14" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="14" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4054,7 +3814,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -4062,7 +3822,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -4174,13 +3934,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4278,7 +4036,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -4286,7 +4044,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -4398,13 +4156,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4502,7 +4258,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -4510,7 +4266,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -4622,13 +4378,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4726,7 +4480,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -4734,7 +4488,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -4846,13 +4600,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4950,7 +4702,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -4958,7 +4710,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -5070,13 +4822,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5174,7 +4924,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -5182,7 +4932,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -5294,13 +5044,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5398,7 +5146,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -5406,7 +5154,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -5518,13 +5266,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5622,7 +5368,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -5630,7 +5376,229 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="14" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>